<commit_message>
Including position_geolabels for lau2
</commit_message>
<xml_diff>
--- a/inst/documentation/fhimaps_ref.xlsx
+++ b/inst/documentation/fhimaps_ref.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riwh\OneDrive - Folkehelseinstituttet\packages\fhimaps\inst\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{D5DD4900-6E52-6940-A96C-8E6545237B55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{D22F1E3D-FAB4-4205-AC1C-7520D7C24FC0}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{D5DD4900-6E52-6940-A96C-8E6545237B55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{A4A996E5-C958-454E-9AA9-0C5533A37859}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F17CE2D-A677-B445-A9FA-8A0D7952F86A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>norway_nuts3_position_geolabels_b2020_insert_oslo_dt</t>
+  </si>
+  <si>
+    <t>norway_lau2_position_geolabels_b2020_default_dt</t>
+  </si>
+  <si>
+    <t>norway_lau2_position_geolabels_b2020_insert_oslo_dt</t>
   </si>
 </sst>
 </file>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC43CB2E-9A09-7A47-86D5-A07830EF818A}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="131" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1048,22 +1054,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" t="s">
         <v>41</v>
@@ -1071,19 +1077,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F24" t="s">
         <v>36</v>
@@ -1094,7 +1100,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -1106,7 +1112,7 @@
         <v>34</v>
       </c>
       <c r="E25">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="F25" t="s">
         <v>36</v>
@@ -1117,22 +1123,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E26">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G26" t="s">
         <v>41</v>
@@ -1140,30 +1146,30 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E27">
         <v>2020</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -1172,15 +1178,61 @@
         <v>31</v>
       </c>
       <c r="D28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28">
+        <v>2020</v>
+      </c>
+      <c r="F28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29">
+        <v>2020</v>
+      </c>
+      <c r="F29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
         <v>33</v>
       </c>
-      <c r="E28">
-        <v>2020</v>
-      </c>
-      <c r="F28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="E30">
+        <v>2020</v>
+      </c>
+      <c r="F30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>